<commit_message>
update: experiment preparation & diary
</commit_message>
<xml_diff>
--- a/Anying Xiang/SEP-B/Sprint 3/Experiment/Experiment Preparation/experiment preparation.xlsx
+++ b/Anying Xiang/SEP-B/Sprint 3/Experiment/Experiment Preparation/experiment preparation.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\G-PostGraduate\SEP-B\Git-Project\Anying Xiang\SEP-B\Sprint 3\Experiment\Preparation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\G-PostGraduate\SEP-B\Git-Project\Anying Xiang\SEP-B\Sprint 3\Experiment\Experiment Preparation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42D5460F-5329-44BA-9AE8-6EA1A88A1B4F}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1131FD0F-AECE-4F6E-8C3C-F68FFF84B7FB}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="74">
   <si>
     <t>Spark Properties</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -200,12 +200,123 @@
     <t>If set to higher value, the burden on memory and cpu might be increased (use more memory, and thus more cpu and disk, memory is the bottleneck).</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
+  <si>
+    <t>search space</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>[1] T. B. G. Perez, W. Chen, R. Ji, L. Liu and X. Zhou, "PETS: Bottleneck-Aware Spark Tuning with Parameter Ensembles," 2018 27th International Conference on Computer Communication and Networks (ICCCN), Hangzhou, 2018, pp. 1-9.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Reference</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Snappy,LZ4,LZF</t>
+  </si>
+  <si>
+    <t>T,F</t>
+  </si>
+  <si>
+    <t>Java, Kryo</t>
+  </si>
+  <si>
+    <t>[2] Gounaris, A. , &amp; Torres, J. . (2017). A methodology for spark parameter tuning. Big Data Research, S2214579617300114.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>8,16,32,64,128 [1]</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Snappy,LZ4,LZF [1]</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>T,F [1]</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Java, Kryo [1]</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1,2,3,4 [1]</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">[3] N. Nguyen, M. Maifi Hasan Khan and K. Wang, "Towards Automatic Tuning of Apache Spark Configuration," 2018 IEEE 11th International Conference on Cloud Computing (CLOUD), San Francisco, CA, 2018, pp. 417-425. </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>12,24,48,96,192 [1]
+72, 24 [2]
+48, 72, 96, 84 [3]</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">0.4, 0.5, 0.6, 0.7, 0.8 [1]
+0.4, 0.5, 0.6, 0.7, 0.8 [3] </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0.3, 0.4, 0.5, 0.6, 0.7 [1]</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>8,16,32,64,128 [1]
+48, 16 [2]
+32, 48, 64 [3]</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1,2,3,4,5 [1]
+6, 7, 8, 9 [3]</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1,2,4,8,16 [1]</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>16, 32, 64</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>24, 48, 72</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>16, 32, 48</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1, 2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2, 4, 8</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1, 3, 5</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0.4, 0.6, 0.8</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0.3, 0.5, 0.7</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -239,8 +350,22 @@
       <name val="等线"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="等线"/>
+      <family val="2"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -263,6 +388,11 @@
       <patternFill patternType="solid">
         <fgColor theme="7" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
       </patternFill>
     </fill>
   </fills>
@@ -316,10 +446,13 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -342,12 +475,31 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
+    <cellStyle name="着色 6" xfId="1" builtinId="49"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -630,10 +782,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B1:I15"/>
+  <dimension ref="B1:K19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I8" sqref="I8"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="J8" sqref="J8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -645,31 +797,35 @@
     <col min="6" max="6" width="10.33203125" customWidth="1"/>
     <col min="7" max="7" width="14.109375" customWidth="1"/>
     <col min="8" max="8" width="14.21875" customWidth="1"/>
-    <col min="9" max="9" width="51.44140625" customWidth="1"/>
-    <col min="10" max="10" width="9.21875" customWidth="1"/>
+    <col min="9" max="9" width="23.109375" customWidth="1"/>
+    <col min="10" max="10" width="14.21875" customWidth="1"/>
+    <col min="11" max="11" width="51.44140625" customWidth="1"/>
+    <col min="12" max="12" width="9.21875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B1" s="7" t="s">
+    <row r="1" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B1" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="7" t="s">
+      <c r="C1" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="6" t="s">
+      <c r="D1" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="E1" s="6"/>
-      <c r="F1" s="6"/>
-      <c r="G1" s="6"/>
+      <c r="E1" s="8"/>
+      <c r="F1" s="8"/>
+      <c r="G1" s="8"/>
       <c r="H1" s="1"/>
-      <c r="I1" s="7" t="s">
+      <c r="I1" s="7"/>
+      <c r="J1" s="7"/>
+      <c r="K1" s="9" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B2" s="8"/>
-      <c r="C2" s="8"/>
+    <row r="2" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B2" s="10"/>
+      <c r="C2" s="10"/>
       <c r="D2" s="1" t="s">
         <v>2</v>
       </c>
@@ -685,9 +841,15 @@
       <c r="H2" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="I2" s="8"/>
-    </row>
-    <row r="3" spans="2:9" ht="41.4" x14ac:dyDescent="0.25">
+      <c r="I2" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="J2" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="K2" s="10"/>
+    </row>
+    <row r="3" spans="2:11" ht="41.4" x14ac:dyDescent="0.25">
       <c r="B3" s="2" t="s">
         <v>10</v>
       </c>
@@ -709,11 +871,17 @@
       <c r="H3" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="I3" s="5" t="s">
+      <c r="I3" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="J3" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="K3" s="5" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="4" spans="2:9" ht="27.6" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:11" ht="27.6" x14ac:dyDescent="0.25">
       <c r="B4" s="2" t="s">
         <v>11</v>
       </c>
@@ -731,11 +899,17 @@
       <c r="H4" s="3" t="b">
         <v>0</v>
       </c>
-      <c r="I4" s="5" t="s">
+      <c r="I4" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="J4" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="K4" s="5" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="5" spans="2:9" ht="27.6" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:11" ht="27.6" x14ac:dyDescent="0.25">
       <c r="B5" s="2" t="s">
         <v>7</v>
       </c>
@@ -753,11 +927,17 @@
       <c r="H5" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="I5" s="5" t="s">
+      <c r="I5" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="J5" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="K5" s="5" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="6" spans="2:9" ht="27.6" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:11" ht="27.6" x14ac:dyDescent="0.25">
       <c r="B6" s="2" t="s">
         <v>42</v>
       </c>
@@ -773,11 +953,17 @@
       <c r="H6" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="I6" s="5" t="s">
+      <c r="I6" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="J6" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="K6" s="5" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="7" spans="2:9" ht="27.6" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:11" ht="27.6" x14ac:dyDescent="0.25">
       <c r="B7" s="2" t="s">
         <v>12</v>
       </c>
@@ -795,11 +981,17 @@
       <c r="H7" s="3" t="b">
         <v>1</v>
       </c>
-      <c r="I7" s="5" t="s">
+      <c r="I7" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="J7" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="K7" s="5" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="8" spans="2:9" ht="41.4" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:11" ht="41.4" x14ac:dyDescent="0.25">
       <c r="B8" s="2" t="s">
         <v>45</v>
       </c>
@@ -819,11 +1011,17 @@
       <c r="H8" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="I8" s="5" t="s">
+      <c r="I8" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="J8" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="K8" s="5" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="9" spans="2:9" ht="41.4" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:11" ht="41.4" x14ac:dyDescent="0.25">
       <c r="B9" s="2" t="s">
         <v>8</v>
       </c>
@@ -841,11 +1039,17 @@
       <c r="H9" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="I9" s="5" t="s">
+      <c r="I9" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="J9" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="K9" s="5" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="10" spans="2:9" ht="27.6" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:11" ht="27.6" x14ac:dyDescent="0.25">
       <c r="B10" s="2" t="s">
         <v>9</v>
       </c>
@@ -863,11 +1067,17 @@
       <c r="H10" s="3" t="b">
         <v>1</v>
       </c>
-      <c r="I10" s="5" t="s">
+      <c r="I10" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="J10" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="K10" s="5" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="11" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B11" s="2" t="s">
         <v>27</v>
       </c>
@@ -885,29 +1095,43 @@
       <c r="H11" s="3">
         <v>1</v>
       </c>
-      <c r="I11" s="5" t="s">
+      <c r="I11" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="J11" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="K11" s="5" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="12" spans="2:9" ht="27.6" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:11" ht="27.6" x14ac:dyDescent="0.25">
       <c r="B12" s="2" t="s">
         <v>35</v>
       </c>
       <c r="C12" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="D12" s="3"/>
+      <c r="D12" s="3" t="s">
+        <v>44</v>
+      </c>
       <c r="E12" s="3"/>
       <c r="F12" s="3"/>
       <c r="G12" s="3"/>
       <c r="H12" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="I12" s="5" t="s">
+      <c r="I12" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="J12" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="K12" s="5" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="13" spans="2:9" ht="27.6" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:11" ht="27.6" x14ac:dyDescent="0.25">
       <c r="B13" s="2" t="s">
         <v>38</v>
       </c>
@@ -925,11 +1149,17 @@
       <c r="H13" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="I13" s="5" t="s">
+      <c r="I13" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="J13" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="K13" s="5" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="14" spans="2:9" ht="41.4" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:11" ht="41.4" x14ac:dyDescent="0.25">
       <c r="B14" s="2" t="s">
         <v>30</v>
       </c>
@@ -947,11 +1177,17 @@
       <c r="H14" s="3">
         <v>0.6</v>
       </c>
-      <c r="I14" s="5" t="s">
+      <c r="I14" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="J14" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="K14" s="5" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="15" spans="2:9" ht="41.4" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:11" ht="41.4" x14ac:dyDescent="0.25">
       <c r="B15" s="2" t="s">
         <v>31</v>
       </c>
@@ -967,16 +1203,70 @@
       <c r="H15" s="3">
         <v>0.5</v>
       </c>
-      <c r="I15" s="5" t="s">
+      <c r="I15" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="J15" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="K15" s="5" t="s">
         <v>34</v>
       </c>
     </row>
+    <row r="17" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B17" s="11" t="s">
+        <v>49</v>
+      </c>
+      <c r="C17" s="12" t="s">
+        <v>48</v>
+      </c>
+      <c r="D17" s="12"/>
+      <c r="E17" s="12"/>
+      <c r="F17" s="12"/>
+      <c r="G17" s="12"/>
+      <c r="H17" s="12"/>
+      <c r="I17" s="12"/>
+      <c r="J17" s="12"/>
+      <c r="K17" s="12"/>
+    </row>
+    <row r="18" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B18" s="11"/>
+      <c r="C18" s="13" t="s">
+        <v>53</v>
+      </c>
+      <c r="D18" s="13"/>
+      <c r="E18" s="13"/>
+      <c r="F18" s="13"/>
+      <c r="G18" s="13"/>
+      <c r="H18" s="13"/>
+      <c r="I18" s="13"/>
+      <c r="J18" s="13"/>
+      <c r="K18" s="13"/>
+    </row>
+    <row r="19" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B19" s="11"/>
+      <c r="C19" s="14" t="s">
+        <v>59</v>
+      </c>
+      <c r="D19" s="14"/>
+      <c r="E19" s="14"/>
+      <c r="F19" s="14"/>
+      <c r="G19" s="14"/>
+      <c r="H19" s="14"/>
+      <c r="I19" s="14"/>
+      <c r="J19" s="14"/>
+      <c r="K19" s="14"/>
+    </row>
   </sheetData>
-  <mergeCells count="4">
+  <mergeCells count="8">
+    <mergeCell ref="C18:K18"/>
+    <mergeCell ref="C19:K19"/>
+    <mergeCell ref="B17:B19"/>
     <mergeCell ref="D1:G1"/>
-    <mergeCell ref="I1:I2"/>
+    <mergeCell ref="K1:K2"/>
     <mergeCell ref="B1:B2"/>
     <mergeCell ref="C1:C2"/>
+    <mergeCell ref="C17:K17"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>